<commit_message>
fix api upload xlxs and entiy DocumentType
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/document_import_template.xlsx
+++ b/src/main/resources/templates/document_import_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Advanced_Programming\Library_Management_System\src\main\resources\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Advanced_Programming\Library_Management_System\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B10F72C-6735-4A4C-A868-25D73FAEBF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DEE113-6F8F-440A-BC31-0339DDE10847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3B7D7997-E147-4716-8893-B2DF2141812F}"/>
   </bookViews>
@@ -83,13 +83,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -103,7 +110,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D8B3F8C9-2DB6-4533-BC5E-FDE91EC24BC7}" name="Table3" displayName="Table3" ref="A1:D1048575" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D8B3F8C9-2DB6-4533-BC5E-FDE91EC24BC7}" name="Table3" displayName="Table3" ref="A1:D1048575" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:D1048575" xr:uid="{D8B3F8C9-2DB6-4533-BC5E-FDE91EC24BC7}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C79B707E-7AB4-477F-BA1F-46BFEF0E092B}" name="Tiêu đề"/>
@@ -435,22 +442,28 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.25" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
+    <col min="3" max="3" width="21.125" customWidth="1"/>
+    <col min="4" max="4" width="16.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add api import from excel
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/document_import_template.xlsx
+++ b/src/main/resources/templates/document_import_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Advanced_Programming\Library_Management_System\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DEE113-6F8F-440A-BC31-0339DDE10847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8F0D00-ABCD-4E7C-B10D-15A03F2226E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3B7D7997-E147-4716-8893-B2DF2141812F}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Tiêu đề</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Tác giả</t>
   </si>
@@ -48,6 +45,27 @@
   </si>
   <si>
     <t>Năm xuất bản</t>
+  </si>
+  <si>
+    <t>Tên tài liệu</t>
+  </si>
+  <si>
+    <t>Số hiệu phân loại</t>
+  </si>
+  <si>
+    <t>Thể loại</t>
+  </si>
+  <si>
+    <t>Vị trí trên kệ</t>
+  </si>
+  <si>
+    <t>Loại tài liệu</t>
+  </si>
+  <si>
+    <t>Liên kết truy cập</t>
+  </si>
+  <si>
+    <t>Trạng thái</t>
   </si>
 </sst>
 </file>
@@ -110,13 +128,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D8B3F8C9-2DB6-4533-BC5E-FDE91EC24BC7}" name="Table3" displayName="Table3" ref="A1:D1048575" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D1048575" xr:uid="{D8B3F8C9-2DB6-4533-BC5E-FDE91EC24BC7}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C79B707E-7AB4-477F-BA1F-46BFEF0E092B}" name="Tiêu đề"/>
-    <tableColumn id="2" xr3:uid="{DD9D4316-231D-47ED-9A47-972A407C2EF8}" name="Tác giả"/>
-    <tableColumn id="3" xr3:uid="{11D44004-4452-4551-8E9C-67735EE16E91}" name="Nhà xuất bản"/>
-    <tableColumn id="4" xr3:uid="{53E9FA29-4BE8-4ADD-9CEC-9BE93EAAD103}" name="Năm xuất bản"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D8B3F8C9-2DB6-4533-BC5E-FDE91EC24BC7}" name="Table3" displayName="Table3" ref="A1:J1048575" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:J1048575" xr:uid="{D8B3F8C9-2DB6-4533-BC5E-FDE91EC24BC7}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{C79B707E-7AB4-477F-BA1F-46BFEF0E092B}" name="Tên tài liệu"/>
+    <tableColumn id="10" xr3:uid="{0BF64929-AEE6-4081-8F5C-CE103D41CE0A}" name="Tác giả"/>
+    <tableColumn id="9" xr3:uid="{0E42235C-7736-4E83-B7C7-88AE150298FD}" name="Nhà xuất bản"/>
+    <tableColumn id="8" xr3:uid="{ED898A6C-14CD-43D0-9817-9F7D2E86B74F}" name="Năm xuất bản"/>
+    <tableColumn id="7" xr3:uid="{902FA56F-AD06-4976-904C-B376E8FE6FF2}" name="Số hiệu phân loại"/>
+    <tableColumn id="6" xr3:uid="{CA023FF0-4FBF-4636-AE7B-1FCE975B2080}" name="Thể loại"/>
+    <tableColumn id="5" xr3:uid="{4D54C098-C167-43A2-93B3-E6912358AF86}" name="Vị trí trên kệ"/>
+    <tableColumn id="2" xr3:uid="{DD9D4316-231D-47ED-9A47-972A407C2EF8}" name="Loại tài liệu"/>
+    <tableColumn id="3" xr3:uid="{11D44004-4452-4551-8E9C-67735EE16E91}" name="Liên kết truy cập"/>
+    <tableColumn id="4" xr3:uid="{53E9FA29-4BE8-4ADD-9CEC-9BE93EAAD103}" name="Trạng thái"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -439,32 +463,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0B913B-6BB1-43EF-BE92-AD843D74C72A}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.25" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="21.125" customWidth="1"/>
-    <col min="4" max="4" width="16.75" customWidth="1"/>
+    <col min="1" max="7" width="24.25" customWidth="1"/>
+    <col min="8" max="8" width="14.875" customWidth="1"/>
+    <col min="9" max="9" width="21.125" customWidth="1"/>
+    <col min="10" max="10" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>